<commit_message>
Integração das listas: Artes, Ciências, Física, Ed. Física, Geografia e História
</commit_message>
<xml_diff>
--- a/ciencias_502.xlsx
+++ b/ciencias_502.xlsx
@@ -11,128 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>RAQUEL CRISTINA DE OLIVEIRA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ELAINE MORAES PINTO ROSSINI</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>JOSÉ ALBERTO MARY VIERA JÚNIOR</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>CLAUDIOMIR DA VEIGA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>MARIA ANGÉLICA VARGAS PINTO DE FARIA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>LUCIMAR DE FREITAS SANTIAGO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ANDREA ALMEIDA SANTANA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ALINE DE OLIVEIRA SOARES RODRIGUES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ALEXANDRE BUZZINARI DE MOURA DIAS JUNIOR</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>WALKIRIA ADILA ACÁCIO REIS</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <rFont val="Times New Roman"/>
-        <b/>
-        <color rgb="FF000009"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>ROBERTA FRANCISCO DE OLIVEIRA MARIANO</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <r>
       <rPr>
@@ -175,6 +54,94 @@
         <sz val="10.0"/>
       </rPr>
       <t>LÍVIA DE ANDRADE LORENÇATO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>FLAVIANA FERREIRA DA VEIGA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>ALINE SODRE AZEVEDO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>JULIANA DA COSTA BENICA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>FERNANDA APARECIDA MONTES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>AMANDA CHAGAS VITOR DE OLIVEIRA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>CASSANDRA ROSA TEIXEIRA GOMES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>CAMILLA MIRANDA RODRIGUES AMARAL</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Times New Roman"/>
+        <b/>
+        <color rgb="FF000009"/>
+        <sz val="10.0"/>
+      </rPr>
+      <t>THIAGO MARTINS BASTOS</t>
     </r>
   </si>
   <si>
@@ -185,6 +152,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="###0;###0"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="10.0"/>
@@ -203,6 +173,7 @@
       <name val="Times New Roman"/>
     </font>
     <font>
+      <b/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -240,15 +211,15 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="1" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="top" wrapText="1"/>
+      <alignment shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+      <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -466,13 +437,12 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="21.63"/>
-    <col customWidth="1" min="2" max="2" width="44.13"/>
+    <col customWidth="1" min="2" max="2" width="38.5"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1">
-        <v>88.0</v>
+        <v>101.0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -480,7 +450,7 @@
     </row>
     <row r="2">
       <c r="A2" s="1">
-        <v>89.0</v>
+        <v>102.0</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>1</v>
@@ -488,7 +458,7 @@
     </row>
     <row r="3">
       <c r="A3" s="1">
-        <v>90.0</v>
+        <v>103.0</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>2</v>
@@ -496,7 +466,7 @@
     </row>
     <row r="4">
       <c r="A4" s="1">
-        <v>92.0</v>
+        <v>104.0</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>3</v>
@@ -504,7 +474,7 @@
     </row>
     <row r="5">
       <c r="A5" s="1">
-        <v>93.0</v>
+        <v>105.0</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>4</v>
@@ -512,7 +482,7 @@
     </row>
     <row r="6">
       <c r="A6" s="1">
-        <v>94.0</v>
+        <v>106.0</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>5</v>
@@ -520,7 +490,7 @@
     </row>
     <row r="7">
       <c r="A7" s="1">
-        <v>95.0</v>
+        <v>107.0</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>6</v>
@@ -528,7 +498,7 @@
     </row>
     <row r="8">
       <c r="A8" s="1">
-        <v>97.0</v>
+        <v>108.0</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>7</v>
@@ -536,7 +506,7 @@
     </row>
     <row r="9">
       <c r="A9" s="1">
-        <v>98.0</v>
+        <v>109.0</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
@@ -544,7 +514,7 @@
     </row>
     <row r="10">
       <c r="A10" s="1">
-        <v>99.0</v>
+        <v>110.0</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>9</v>
@@ -552,7 +522,7 @@
     </row>
     <row r="11">
       <c r="A11" s="1">
-        <v>100.0</v>
+        <v>111.0</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
@@ -560,40 +530,16 @@
     </row>
     <row r="12">
       <c r="A12" s="1">
-        <v>101.0</v>
+        <v>112.0</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1">
-        <v>102.0</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="A13" s="3"/>
+      <c r="B13" s="4" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="1">
-        <v>103.0</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="1">
-        <v>104.0</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adição 499 e 502
</commit_message>
<xml_diff>
--- a/ciencias_502.xlsx
+++ b/ciencias_502.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="15" windowWidth="18960" windowHeight="11325"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12735"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -14,116 +14,184 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000009"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>MAÍRA TORMEN DE SOUZA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color rgb="FF000009"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>EXCEDENTES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000009"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>MICHELLE CLEMENTE DE OLIVEIRA SOUZA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000009"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>THAIS SILVA MARTINS MEDEIROS</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000009"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>VANESSA SANTOS VALLE COSTA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000009"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>CECILIA MARIA DA FONSECA RIBEIRO MAGALHÃES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000009"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>PATRÍCIA ALVES DE MENDONÇA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000009"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>CAROLINA UMBELINO DE MAGALHAES</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000009"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>ERIKA GONÇALVES DE OLIVEIRA MARQUES</t>
-    </r>
-  </si>
-  <si>
-    <t>FIM - CIÊNCIAS</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000009"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>MARCUS VINICIUS MARTINS DIAS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000009"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>CINTIA FERREIRA DIAS</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000009"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>FERNANDA BELLI MIRANDA MENDES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000009"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>INGRID SANTOS OLIVEIRA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000009"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>DANIELE PEREIRA DA SILVA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000009"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>LAYZE FERNANDA DOS SANTOS NICÁCIO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000009"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>DAYANA MARTINS DA ROCHA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000009"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>JUSSARA DE OLIVEIRA PAULA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000009"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>PABLO DE MAGALHAES</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000009"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>FELIPE AUGUSTO DA SILVA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000009"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>MYLENA CHRISTINA FERNANDES PEREIRA</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000009"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>GESSYCA BAGIO GROSSO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000009"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ARTHUR PONTÉ RINCO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000009"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>MAÍRA ARAÚJO AZEVEDO</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000009"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>ADENILCE APARECIDA DA SILVA SOUZA</t>
+    </r>
+  </si>
+  <si>
+    <t>Fim Ciências</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="###0;###0"/>
+  </numFmts>
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -131,48 +199,25 @@
       <charset val="204"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000009"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000009"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000009"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCCCCC"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -184,21 +229,6 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
       <right/>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -215,6 +245,32 @@
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
       </top>
       <bottom style="thin">
         <color rgb="FF000000"/>
@@ -225,21 +281,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -250,6 +312,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -542,98 +607,162 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.33203125" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
-    <col min="2" max="2" width="74.1640625" customWidth="1"/>
-    <col min="3" max="3" width="3.83203125" customWidth="1"/>
+    <col min="1" max="1" width="16.1640625" customWidth="1"/>
+    <col min="2" max="2" width="14" customWidth="1"/>
+    <col min="3" max="3" width="58.1640625" customWidth="1"/>
+    <col min="4" max="6" width="1.1640625" customWidth="1"/>
+    <col min="7" max="7" width="2.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2">
-        <v>113</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:3" ht="27" customHeight="1">
+      <c r="A1" s="1">
+        <v>121</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="24.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" ht="27" customHeight="1">
+      <c r="A2" s="4">
+        <v>122</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-    </row>
-    <row r="3" spans="1:2" ht="24.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>114</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="C2" s="6"/>
+    </row>
+    <row r="3" spans="1:3" ht="27" customHeight="1">
+      <c r="A3" s="1">
+        <v>123</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" ht="24.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
-        <v>115</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="C3" s="3"/>
+    </row>
+    <row r="4" spans="1:3" ht="27" customHeight="1">
+      <c r="A4" s="4">
+        <v>124</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" ht="24.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
-        <v>116</v>
-      </c>
-      <c r="B5" s="1" t="s">
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" ht="27" customHeight="1">
+      <c r="A5" s="4">
+        <v>125</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" ht="24.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
-        <v>117</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C5" s="6"/>
+    </row>
+    <row r="6" spans="1:3" ht="27" customHeight="1">
+      <c r="A6" s="4">
+        <v>126</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="24.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
-        <v>118</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="C6" s="6"/>
+    </row>
+    <row r="7" spans="1:3" ht="27" customHeight="1">
+      <c r="A7" s="4">
+        <v>127</v>
+      </c>
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" ht="24.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
-        <v>119</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C7" s="6"/>
+    </row>
+    <row r="8" spans="1:3" ht="27" customHeight="1">
+      <c r="A8" s="4">
+        <v>128</v>
+      </c>
+      <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="24.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
-        <v>120</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="C8" s="6"/>
+    </row>
+    <row r="9" spans="1:3" ht="27" customHeight="1">
+      <c r="A9" s="4">
+        <v>129</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B10" t="s">
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" ht="27" customHeight="1">
+      <c r="A10" s="4">
+        <v>130</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
+      <c r="C10" s="6"/>
+    </row>
+    <row r="11" spans="1:3" ht="27" customHeight="1">
+      <c r="A11" s="4">
+        <v>131</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" ht="27" customHeight="1">
+      <c r="A12" s="4">
+        <v>132</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" ht="27" customHeight="1">
+      <c r="A13" s="4">
+        <v>133</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" ht="27" customHeight="1">
+      <c r="A14" s="4">
+        <v>134</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="6"/>
+    </row>
+    <row r="15" spans="1:3" ht="27" customHeight="1">
+      <c r="A15" s="4">
+        <v>135</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:B2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>